<commit_message>
adding results with the whole dataset
</commit_message>
<xml_diff>
--- a/datasets/dataset-ragas-openai-2.xlsx
+++ b/datasets/dataset-ragas-openai-2.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB3D6E3-7F9A-4254-8A51-24477D19A849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5BAD73-4AF7-4D29-91BD-1B3BBD4A3AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{B82DB73C-14D7-482A-AD66-E9CA90FE2CC9}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="38700" windowHeight="15885" xr2:uid="{B82DB73C-14D7-482A-AD66-E9CA90FE2CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset-ragas-openai-edital1" sheetId="2" r:id="rId1"/>
     <sheet name="dataset-ragas-openai-edital2" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">'dataset-ragas-openai-edital1'!$A$1:$C$29</definedName>
+    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">'dataset-ragas-openai-edital1'!$A$1:$C$28</definedName>
     <definedName name="DadosExternos_1" localSheetId="1" hidden="1">'dataset-ragas-openai-edital2'!$A$1:$C$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="108">
   <si>
     <t>user_input</t>
   </si>
@@ -82,12 +82,6 @@
   </si>
   <si>
     <t>A Pro-Reitoria de Assuntos Estudantis - Proaes é responsável por tornar público o Edital PROAES/UFMS Nº 70, que estabelece as normas para o cadastro de estudantes de graduação indígenas e quilombolas para a concessão de Bolsa Permanência do MEC - BPMEC. Ela atua no uso de suas atribuições legais e de acordo com as Portarias MEC que regulamentam o programa.</t>
-  </si>
-  <si>
-    <t>O que é a FUNDAÇÃO UNIVERSIDADE FEDERAL DE MATO GROSSO DO SUL e qual é o objetivo do Edital PROAES/UFMS Nº 70?</t>
-  </si>
-  <si>
-    <t>A FUNDAÇÃO UNIVERSIDADE FEDERAL DE MATO GROSSO DO SUL, por meio da Pró-Reitoria de Assuntos Estudantis - Proaes, publica o Edital PROAES/UFMS Nº 70 com o objetivo de estabelecer as normas para o cadastro de estudantes de graduação indígenas e quilombolas para a concessão de Bolsa Permanência do MEC - BPMEC.</t>
   </si>
   <si>
     <t>Qual é a finalidade da Bolsa Permanência do MEC conforme descrito no edital PROAES/UFMS Nº 70, DE 4 DE JUNHO DE 2024?</t>
@@ -495,8 +489,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5EDE1C51-8888-4E77-9842-D991FC8BA3C5}" name="dataset_ragas_openai_edital1" displayName="dataset_ragas_openai_edital1" ref="A1:D29" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D29" xr:uid="{5EDE1C51-8888-4E77-9842-D991FC8BA3C5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5EDE1C51-8888-4E77-9842-D991FC8BA3C5}" name="dataset_ragas_openai_edital1" displayName="dataset_ragas_openai_edital1" ref="A1:D28" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D28" xr:uid="{5EDE1C51-8888-4E77-9842-D991FC8BA3C5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B50E08F4-D9AB-4589-839A-7E3463C15E09}" uniqueName="1" name="user_input" queryTableFieldId="1" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{C7948349-B236-4E4D-B631-4F26D621EE99}" uniqueName="2" name="reference" queryTableFieldId="2" dataDxfId="6"/>
@@ -837,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC780454-6F00-446A-A281-1FECFFECBC73}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +853,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -884,7 +878,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -899,28 +893,28 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -934,96 +928,93 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>109</v>
+      <c r="C14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,60 +1025,63 @@
         <v>31</v>
       </c>
       <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1095,52 +1089,52 @@
         <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" t="s">
-        <v>109</v>
+      <c r="C21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>42</v>
+      <c r="D22" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,35 +1145,35 @@
         <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" t="s">
-        <v>109</v>
+      <c r="C25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
-        <v>42</v>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1190,10 +1184,10 @@
         <v>51</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1204,24 +1198,10 @@
         <v>53</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1236,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC04BC5-0F91-4321-B582-2B2E88389B87}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:D25"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,273 +1236,273 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
         <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
         <v>73</v>
-      </c>
-      <c r="B11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
         <v>78</v>
-      </c>
-      <c r="B14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
         <v>85</v>
-      </c>
-      <c r="B17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="D19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
         <v>97</v>
-      </c>
-      <c r="B22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>